<commit_message>
Added new plotting data from ADS.
</commit_message>
<xml_diff>
--- a/Correlations.xlsx
+++ b/Correlations.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="986" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="15150" tabRatio="986" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="MLIN_Slot_Circular" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -451,7 +451,7 @@
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -466,7 +466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,6 +490,11 @@
           <t>S11_CST</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>S11_ADS_FEM</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -506,6 +511,9 @@
       <c r="D2" t="n">
         <v>-0.582502324943327</v>
       </c>
+      <c r="E2" t="n">
+        <v>-0.6501231965313155</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -522,6 +530,9 @@
       <c r="D3" t="n">
         <v>0.7481788943675789</v>
       </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -536,6 +547,22 @@
         <v>0.7481788943675789</v>
       </c>
       <c r="D4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>S11_ADS_FEM</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-0.6501231965313155</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1054,7 +1081,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1078,6 +1105,11 @@
           <t>S11_CST</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>S11_ADS_FEM</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -1094,6 +1126,9 @@
       <c r="D2" t="n">
         <v>-0.8322610138323583</v>
       </c>
+      <c r="E2" t="n">
+        <v>-0.4036618505910266</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -1110,6 +1145,9 @@
       <c r="D3" t="n">
         <v>0.3324880639301741</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.9999999999999999</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -1124,6 +1162,22 @@
         <v>0.3324880639301741</v>
       </c>
       <c r="D4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>S11_ADS_FEM</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-0.4036618505910266</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.9999999999999999</v>
+      </c>
+      <c r="E5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1173,7 +1227,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.111463287315364</v>
+        <v>-0.5015996501889113</v>
       </c>
       <c r="D2" t="n">
         <v>-0.3786692998336854</v>
@@ -1186,13 +1240,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.111463287315364</v>
+        <v>-0.5015996501889113</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9899812907009593</v>
+        <v>-0.3896835492505257</v>
       </c>
     </row>
     <row r="4">
@@ -1205,7 +1259,7 @@
         <v>-0.3786692998336854</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9899812907009593</v>
+        <v>-0.3896835492505257</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
@@ -1341,7 +1395,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.404847516455586</v>
+        <v>0.4479707490939402</v>
       </c>
       <c r="D2" t="n">
         <v>-0.2852497326357801</v>
@@ -1354,13 +1408,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.404847516455586</v>
+        <v>0.4479707490939402</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8992612562517348</v>
+        <v>0.8673387799484744</v>
       </c>
     </row>
     <row r="4">
@@ -1373,7 +1427,7 @@
         <v>-0.2852497326357801</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8992612562517348</v>
+        <v>0.8673387799484744</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Cardioid and Koch Parametrics Plots
</commit_message>
<xml_diff>
--- a/Correlations.xlsx
+++ b/Correlations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srezende\Desktop\Coding &amp; Programing\S11_Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding and Programing\S11_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C3BE7C-5D4F-4AC8-80EB-26B4C771EC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E77FC5-F3B4-4222-9CF3-F4F3805C2550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29265" yWindow="540" windowWidth="17280" windowHeight="9075" tabRatio="986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ganho" sheetId="1" r:id="rId1"/>
@@ -421,15 +421,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -437,59 +437,43 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>-0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>9</v>
+        <v>12.5</v>
       </c>
       <c r="B5">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B6">
-        <v>-0.8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>12.5</v>
-      </c>
-      <c r="B7">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>14</v>
-      </c>
-      <c r="B8">
         <v>0.4</v>
       </c>
     </row>
@@ -504,9 +488,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,7 +504,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -537,7 +521,7 @@
         <v>-0.65012319653131545</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -554,7 +538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -568,7 +552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -593,9 +577,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -606,7 +590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -620,7 +604,7 @@
         <v>-0.52572820105575147</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -634,7 +618,7 @@
         <v>0.66952974051083025</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -659,9 +643,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -672,7 +656,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -686,7 +670,7 @@
         <v>0.1236733230272109</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -700,7 +684,7 @@
         <v>-0.35869021658925859</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -725,9 +709,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -738,7 +722,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -752,7 +736,7 @@
         <v>1.4274828601012359E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -766,7 +750,7 @@
         <v>-0.24260018201919181</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -791,9 +775,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -804,7 +788,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -818,7 +802,7 @@
         <v>-0.42448612468305419</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -832,7 +816,7 @@
         <v>0.79852396475859433</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -857,9 +841,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -870,7 +854,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -884,7 +868,7 @@
         <v>-0.54890054156007784</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -898,7 +882,7 @@
         <v>0.50211124622787173</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -923,9 +907,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -936,7 +920,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -950,7 +934,7 @@
         <v>-0.36334279051565482</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -964,7 +948,7 @@
         <v>0.88771363905278955</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -989,9 +973,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1005,7 +989,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1022,7 +1006,7 @@
         <v>-0.40366185059102661</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1039,7 +1023,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1053,7 +1037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1078,9 +1062,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1091,7 +1075,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1105,7 +1089,7 @@
         <v>-0.37866929983368541</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1119,7 +1103,7 @@
         <v>-0.38968354925052567</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1144,9 +1128,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1157,7 +1141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1171,7 +1155,7 @@
         <v>-4.1096581447310918E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1185,7 +1169,7 @@
         <v>0.78751938737865446</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1210,9 +1194,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1223,7 +1207,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1237,7 +1221,7 @@
         <v>-0.28524973263578007</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1251,7 +1235,7 @@
         <v>0.86733877994847441</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1276,9 +1260,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1289,7 +1273,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1303,7 +1287,7 @@
         <v>-0.33892291391774099</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1317,7 +1301,7 @@
         <v>0.82238573077369759</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>